<commit_message>
Setting up demonstration for MEEM team
</commit_message>
<xml_diff>
--- a/data/rogers_data_master.xlsx
+++ b/data/rogers_data_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/beesech_staff_vuw_ac_nz/Documents/Thesis/3_mizerReef/mizerReef/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{252141C0-194E-400D-B46C-018D7CB89B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9ED5F91-702B-4936-B8FE-0BFF306F41AB}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{252141C0-194E-400D-B46C-018D7CB89B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0ABCFEB-889B-4901-8914-373462A298F1}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{925FE84C-6781-4A62-93C2-5A8DAACE6349}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{925FE84C-6781-4A62-93C2-5A8DAACE6349}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>algae</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>biomass_observed</t>
+  </si>
+  <si>
+    <t>biomass_cutoff</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -450,15 +459,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BCE1E66-B023-4013-B5DB-B7E603FD1305}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -469,37 +495,43 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -510,37 +542,43 @@
         <v>3.1622776999999998E-2</v>
       </c>
       <c r="D2">
+        <v>107.269812380122</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
         <v>0.1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>3</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>100</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>6.4</v>
       </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
       <c r="M2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -551,37 +589,43 @@
         <v>3.1622776999999998E-2</v>
       </c>
       <c r="D3">
+        <v>33.793040863225002</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
         <v>0.15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>0.2</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
       <c r="M3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -591,34 +635,40 @@
       <c r="C4">
         <v>1E-4</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
         <v>0.15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>100</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>0.2</v>
       </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
       <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>